<commit_message>
Thêm CV mẫu từ website cvtips.com
</commit_message>
<xml_diff>
--- a/Documents/Requirements/Profiles vs. Job Requirements.xlsx
+++ b/Documents/Requirements/Profiles vs. Job Requirements.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="480" yWindow="120" windowWidth="10515" windowHeight="4680"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Profiles" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -19,7 +19,7 @@
     <author>Trung Hieu</author>
   </authors>
   <commentList>
-    <comment ref="A13" authorId="0">
+    <comment ref="A20" authorId="0">
       <text>
         <r>
           <rPr>
@@ -49,7 +49,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A17" authorId="0">
+    <comment ref="A24" authorId="0">
       <text>
         <r>
           <rPr>
@@ -85,6 +85,40 @@
 Projects / Activities:
 Description
 Experiences (you did you learned)
+Who did you report to?
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A32" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Trung Hieu:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+May be:
+- Career opportunities
+- New ventures
+- Expertise Requests
+- Reference requests
+- Consulting offers
+- Job inquiries
+- Business deals
+- Getting back in touch
 </t>
         </r>
       </text>
@@ -94,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Personal Info</t>
   </si>
@@ -127,9 +161,6 @@
   </si>
   <si>
     <t xml:space="preserve"> - Kinh nghiệm làm việc (động nếu ứng viên không thực hiện theo dự án)</t>
-  </si>
-  <si>
-    <t>Skills</t>
   </si>
   <si>
     <t>Recommend actions</t>
@@ -193,9 +224,6 @@
     <t>- Yêu cầu về mối quan hệ</t>
   </si>
   <si>
-    <t>- Archivements</t>
-  </si>
-  <si>
     <t>Educations &amp; Knowledges</t>
   </si>
   <si>
@@ -209,6 +237,27 @@
   </si>
   <si>
     <t>Applications (Facebook, Google+, Twitter…)</t>
+  </si>
+  <si>
+    <t>Additional Information</t>
+  </si>
+  <si>
+    <t>Websites</t>
+  </si>
+  <si>
+    <t>Twitter</t>
+  </si>
+  <si>
+    <t>Interests</t>
+  </si>
+  <si>
+    <t>Groups and Associations</t>
+  </si>
+  <si>
+    <t>Honors and Awards</t>
+  </si>
+  <si>
+    <t>Skills / Abilities</t>
   </si>
 </sst>
 </file>
@@ -607,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:B37"/>
+  <dimension ref="A3:B44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,10 +670,10 @@
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -642,7 +691,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -650,12 +699,12 @@
         <v>3</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B9" s="7"/>
     </row>
@@ -664,148 +713,176 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B12" t="s">
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="B36" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B14" t="s">
+    </row>
+    <row r="39" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="8"/>
+      <c r="B39" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="6"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>